<commit_message>
misc improvements, versioned 1.0.6
</commit_message>
<xml_diff>
--- a/yamf-examples/sample-reports/example-acceptancetests-marks-submission1.xlsx
+++ b/yamf-examples/sample-reports/example-acceptancetests-marks-submission1.xlsx
@@ -9,14 +9,12 @@
     <sheet name="results" r:id="rId3" sheetId="1"/>
     <sheet name="details-1" r:id="rId4" sheetId="2"/>
     <sheet name="details-2" r:id="rId5" sheetId="3"/>
-    <sheet name="details-3" r:id="rId6" sheetId="4"/>
-    <sheet name="details-4" r:id="rId7" sheetId="5"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="151">
   <si>
     <t>task</t>
   </si>
@@ -42,7 +40,7 @@
     <t>ok</t>
   </si>
   <si>
-    <t>details-1,details-2</t>
+    <t>details-1</t>
   </si>
   <si>
     <t>Q2 -- run advanced acceptance tests to check overflow handing</t>
@@ -51,7 +49,7 @@
     <t>fail</t>
   </si>
   <si>
-    <t>details-3,details-4</t>
+    <t>details-2</t>
   </si>
   <si>
     <t>summary</t>
@@ -66,7 +64,7 @@
     <t>&lt;?xml version="1.0" encoding="UTF-8"?&gt;</t>
   </si>
   <si>
-    <t>&lt;testsuite name="JUnit Jupiter" tests="3" skipped="0" failures="0" errors="0" time="0.042" hostname="jens" timestamp="2020-06-12T20:49:20"&gt;</t>
+    <t>&lt;testsuite name="JUnit Jupiter" tests="3" skipped="0" failures="0" errors="0" time="0.048" hostname="jens" timestamp="2020-06-15T13:21:52"&gt;</t>
   </si>
   <si>
     <t>&lt;properties&gt;</t>
@@ -207,7 +205,7 @@
     <t>&lt;property name="sun.io.unicode.encoding" value="UnicodeBig"/&gt;</t>
   </si>
   <si>
-    <t>&lt;property name="sun.java.command" value="/Users/jens/Development/yamf/yamf-core/target/classes/junit-platform-console-standalone-1.6.2.jar -reports-dir /Users/jens/Development/yamf/.junit-reports/2020-06-12--20-49-19--752 -cp /Users/jens/.m2/repository/org/junit/jupiter/junit-jupiter-engine/5.6.2/junit-jupiter-engine-5.6.2.jar:/Users/jens/.m2/repository/org/apiguardian/apiguardian-api/1.1.0/apiguardian-api-1.1.0.jar:/Users/jens/.m2/repository/org/junit/platform/junit-platform-engine/1.6.2/junit-platform-engine-1.6.2.jar:/Users/jens/.m2/repository/org/opentest4j/opentest4j/1.2.0/opentest4j-1.2.0.jar:/Users/jens/.m2/repository/org/junit/platform/junit-platform-commons/1.6.2/junit-platform-commons-1.6.2.jar:/Users/jens/.m2/repository/org/junit/jupiter/junit-jupiter-api/5.6.2/junit-jupiter-api-5.6.2.jar:/Users/jens/Development/yamf/yamf-examples/examples/acceptancetests/reference-solution-with-tests/target/test-classes:/Users/jens/Development/yamf/yamf-examples/examples/acceptancetests/submissions/submission1/target/classes -c acceptancetests.TestCalculatorSimple"/&gt;</t>
+    <t>&lt;property name="sun.java.command" value="/Users/jens/Development/yamf/yamf-core/target/classes/junit-platform-console-standalone-1.6.2.jar -reports-dir /Users/jens/Development/yamf/.junit-reports/2020-06-15--13-21-51--572 -cp /Users/jens/.m2/repository/org/junit/jupiter/junit-jupiter-engine/5.6.2/junit-jupiter-engine-5.6.2.jar:/Users/jens/.m2/repository/org/apiguardian/apiguardian-api/1.1.0/apiguardian-api-1.1.0.jar:/Users/jens/.m2/repository/org/junit/platform/junit-platform-engine/1.6.2/junit-platform-engine-1.6.2.jar:/Users/jens/.m2/repository/org/opentest4j/opentest4j/1.2.0/opentest4j-1.2.0.jar:/Users/jens/.m2/repository/org/junit/platform/junit-platform-commons/1.6.2/junit-platform-commons-1.6.2.jar:/Users/jens/.m2/repository/org/junit/jupiter/junit-jupiter-api/5.6.2/junit-jupiter-api-5.6.2.jar:/Users/jens/Development/yamf/yamf-examples/examples/acceptancetests/reference-solution-with-tests/target/test-classes:/Users/jens/Development/yamf/yamf-examples/examples/acceptancetests/submissions/submission1/target/classes -c acceptancetests.TestCalculatorSimple"/&gt;</t>
   </si>
   <si>
     <t>&lt;property name="sun.java.launcher" value="SUN_STANDARD"/&gt;</t>
@@ -243,7 +241,7 @@
     <t>&lt;/properties&gt;</t>
   </si>
   <si>
-    <t>&lt;testcase name="test1()" classname="acceptancetests.TestCalculatorSimple" time="0.015"&gt;</t>
+    <t>&lt;testcase name="test1()" classname="acceptancetests.TestCalculatorSimple" time="0.017"&gt;</t>
   </si>
   <si>
     <t>&lt;system-out&gt;&lt;![CDATA[</t>
@@ -288,25 +286,13 @@
     <t>&lt;/testsuite&gt;</t>
   </si>
   <si>
-    <t>TEST-junit-vintage.xml</t>
-  </si>
-  <si>
-    <t>&lt;testsuite name="JUnit Vintage" tests="0" skipped="0" failures="0" errors="0" time="0.001" hostname="jens" timestamp="2020-06-12T20:49:20"&gt;</t>
-  </si>
-  <si>
-    <t>unique-id: [engine:junit-vintage]</t>
-  </si>
-  <si>
-    <t>display-name: JUnit Vintage</t>
-  </si>
-  <si>
-    <t>&lt;testsuite name="JUnit Jupiter" tests="1" skipped="0" failures="1" errors="0" time="0.038" hostname="jens" timestamp="2020-06-12T20:49:26"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;property name="sun.java.command" value="/Users/jens/Development/yamf/yamf-core/target/classes/junit-platform-console-standalone-1.6.2.jar -reports-dir /Users/jens/Development/yamf/.junit-reports/2020-06-12--20-49-25--897 -cp /Users/jens/.m2/repository/org/junit/jupiter/junit-jupiter-engine/5.6.2/junit-jupiter-engine-5.6.2.jar:/Users/jens/.m2/repository/org/apiguardian/apiguardian-api/1.1.0/apiguardian-api-1.1.0.jar:/Users/jens/.m2/repository/org/junit/platform/junit-platform-engine/1.6.2/junit-platform-engine-1.6.2.jar:/Users/jens/.m2/repository/org/opentest4j/opentest4j/1.2.0/opentest4j-1.2.0.jar:/Users/jens/.m2/repository/org/junit/platform/junit-platform-commons/1.6.2/junit-platform-commons-1.6.2.jar:/Users/jens/.m2/repository/org/junit/jupiter/junit-jupiter-api/5.6.2/junit-jupiter-api-5.6.2.jar:/Users/jens/Development/yamf/yamf-examples/examples/acceptancetests/reference-solution-with-tests/target/test-classes:/Users/jens/Development/yamf/yamf-examples/examples/acceptancetests/submissions/submission1/target/classes -c acceptancetests.TestCalculatorOverflow"/&gt;</t>
-  </si>
-  <si>
-    <t>&lt;testcase name="testOverflow()" classname="acceptancetests.TestCalculatorOverflow" time="0.014"&gt;</t>
+    <t>&lt;testsuite name="JUnit Jupiter" tests="1" skipped="0" failures="1" errors="0" time="0.05" hostname="jens" timestamp="2020-06-15T13:21:58"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;property name="sun.java.command" value="/Users/jens/Development/yamf/yamf-core/target/classes/junit-platform-console-standalone-1.6.2.jar -reports-dir /Users/jens/Development/yamf/.junit-reports/2020-06-15--13-21-58--080 -cp /Users/jens/.m2/repository/org/junit/jupiter/junit-jupiter-engine/5.6.2/junit-jupiter-engine-5.6.2.jar:/Users/jens/.m2/repository/org/apiguardian/apiguardian-api/1.1.0/apiguardian-api-1.1.0.jar:/Users/jens/.m2/repository/org/junit/platform/junit-platform-engine/1.6.2/junit-platform-engine-1.6.2.jar:/Users/jens/.m2/repository/org/opentest4j/opentest4j/1.2.0/opentest4j-1.2.0.jar:/Users/jens/.m2/repository/org/junit/platform/junit-platform-commons/1.6.2/junit-platform-commons-1.6.2.jar:/Users/jens/.m2/repository/org/junit/jupiter/junit-jupiter-api/5.6.2/junit-jupiter-api-5.6.2.jar:/Users/jens/Development/yamf/yamf-examples/examples/acceptancetests/reference-solution-with-tests/target/test-classes:/Users/jens/Development/yamf/yamf-examples/examples/acceptancetests/submissions/submission1/target/classes -c acceptancetests.TestCalculatorOverflow"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;testcase name="testOverflow()" classname="acceptancetests.TestCalculatorOverflow" time="0.019"&gt;</t>
   </si>
   <si>
     <t>&lt;failure message="Expected java.lang.IllegalArgumentException to be thrown, but nothing was thrown." type="org.opentest4j.AssertionFailedError"&gt;&lt;![CDATA[org.opentest4j.AssertionFailedError: Expected java.lang.IllegalArgumentException to be thrown, but nothing was thrown.</t>
@@ -481,9 +467,6 @@
   </si>
   <si>
     <t>display-name: testOverflow()</t>
-  </si>
-  <si>
-    <t>&lt;testsuite name="JUnit Vintage" tests="0" skipped="0" failures="0" errors="0" time="0.001" hostname="jens" timestamp="2020-06-12T20:49:26"&gt;</t>
   </si>
 </sst>
 </file>
@@ -491,33 +474,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="20">
+  <fonts count="16">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="12.0"/>
-      <color indexed="8"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -634,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center" horizontal="center"/>
@@ -681,18 +644,6 @@
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true">
       <alignment vertical="center" horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center" horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center" horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center" horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFill="true" applyFont="true">
-      <alignment vertical="center" horizontal="left"/>
-    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -710,7 +661,7 @@
     <col min="3" max="3" width="7.1171875" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="11.171875" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="6.4921875" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="19.41796875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="9.9609375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -780,8 +731,9 @@
         <f>C2+C3</f>
         <v>0.0</v>
       </c>
-      <c r="D4" t="s" s="10">
-        <v>13</v>
+      <c r="D4" t="n" s="11">
+        <f>D2+D3</f>
+        <v>0.0</v>
       </c>
       <c r="E4" t="s" s="10">
         <v>13</v>
@@ -1233,7 +1185,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A66"/>
+  <dimension ref="A1:A147"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1244,7 +1196,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="14">
-        <v>90</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -1254,7 +1206,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="15">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4">
@@ -1489,7 +1441,7 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="15">
-        <v>63</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51">
@@ -1549,1123 +1501,431 @@
     </row>
     <row r="62">
       <c r="A62" t="s" s="15">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="15">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s" s="15">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s" s="15">
-        <v>79</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s" s="15">
-        <v>89</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A147"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="255.0" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="17">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="17">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="17">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="17">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="17">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="17">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="17">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="17">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="17">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="17">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="17">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="17">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="17">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="17">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="17">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="17">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="17">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="17">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="17">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="17">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="17">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="17">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="17">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="17">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="17">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="17">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="17">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="17">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="17">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="17">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="17">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="17">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="17">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="17">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="17">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="17">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="17">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="17">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="17">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="17">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="17">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="17">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="17">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="17">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="17">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="17">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="17">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="17">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="17">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s" s="17">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s" s="17">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s" s="17">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s" s="17">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s" s="17">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="17">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="17">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s" s="17">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s" s="17">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s" s="17">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="17">
         <v>96</v>
       </c>
     </row>
-    <row r="63">
-      <c r="A63" t="s" s="17">
+    <row r="67">
+      <c r="A67" t="s" s="15">
         <v>97</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="s" s="17">
+    <row r="68">
+      <c r="A68" t="s" s="15">
         <v>98</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="s" s="17">
+    <row r="69">
+      <c r="A69" t="s" s="15">
         <v>99</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="s" s="17">
+    <row r="70">
+      <c r="A70" t="s" s="15">
         <v>100</v>
       </c>
     </row>
-    <row r="67">
-      <c r="A67" t="s" s="17">
+    <row r="71">
+      <c r="A71" t="s" s="15">
         <v>101</v>
       </c>
     </row>
-    <row r="68">
-      <c r="A68" t="s" s="17">
+    <row r="72">
+      <c r="A72" t="s" s="15">
         <v>102</v>
       </c>
     </row>
-    <row r="69">
-      <c r="A69" t="s" s="17">
+    <row r="73">
+      <c r="A73" t="s" s="15">
         <v>103</v>
       </c>
     </row>
-    <row r="70">
-      <c r="A70" t="s" s="17">
+    <row r="74">
+      <c r="A74" t="s" s="15">
         <v>104</v>
       </c>
     </row>
-    <row r="71">
-      <c r="A71" t="s" s="17">
+    <row r="75">
+      <c r="A75" t="s" s="15">
         <v>105</v>
       </c>
     </row>
-    <row r="72">
-      <c r="A72" t="s" s="17">
+    <row r="76">
+      <c r="A76" t="s" s="15">
         <v>106</v>
       </c>
     </row>
-    <row r="73">
-      <c r="A73" t="s" s="17">
+    <row r="77">
+      <c r="A77" t="s" s="15">
         <v>107</v>
       </c>
     </row>
-    <row r="74">
-      <c r="A74" t="s" s="17">
+    <row r="78">
+      <c r="A78" t="s" s="15">
         <v>108</v>
       </c>
     </row>
-    <row r="75">
-      <c r="A75" t="s" s="17">
+    <row r="79">
+      <c r="A79" t="s" s="15">
         <v>109</v>
       </c>
     </row>
-    <row r="76">
-      <c r="A76" t="s" s="17">
+    <row r="80">
+      <c r="A80" t="s" s="15">
         <v>110</v>
       </c>
     </row>
-    <row r="77">
-      <c r="A77" t="s" s="17">
+    <row r="81">
+      <c r="A81" t="s" s="15">
         <v>111</v>
       </c>
     </row>
-    <row r="78">
-      <c r="A78" t="s" s="17">
+    <row r="82">
+      <c r="A82" t="s" s="15">
         <v>112</v>
       </c>
     </row>
-    <row r="79">
-      <c r="A79" t="s" s="17">
+    <row r="83">
+      <c r="A83" t="s" s="15">
         <v>113</v>
       </c>
     </row>
-    <row r="80">
-      <c r="A80" t="s" s="17">
+    <row r="84">
+      <c r="A84" t="s" s="15">
         <v>114</v>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" t="s" s="17">
+    <row r="85">
+      <c r="A85" t="s" s="15">
         <v>115</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" t="s" s="17">
+    <row r="86">
+      <c r="A86" t="s" s="15">
         <v>116</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="s" s="17">
+    <row r="87">
+      <c r="A87" t="s" s="15">
         <v>117</v>
       </c>
     </row>
-    <row r="84">
-      <c r="A84" t="s" s="17">
+    <row r="88">
+      <c r="A88" t="s" s="15">
         <v>118</v>
       </c>
     </row>
-    <row r="85">
-      <c r="A85" t="s" s="17">
+    <row r="89">
+      <c r="A89" t="s" s="15">
         <v>119</v>
       </c>
     </row>
-    <row r="86">
-      <c r="A86" t="s" s="17">
+    <row r="90">
+      <c r="A90" t="s" s="15">
         <v>120</v>
       </c>
     </row>
-    <row r="87">
-      <c r="A87" t="s" s="17">
+    <row r="91">
+      <c r="A91" t="s" s="15">
         <v>121</v>
       </c>
     </row>
-    <row r="88">
-      <c r="A88" t="s" s="17">
+    <row r="92">
+      <c r="A92" t="s" s="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s" s="15">
         <v>122</v>
       </c>
     </row>
-    <row r="89">
-      <c r="A89" t="s" s="17">
+    <row r="94">
+      <c r="A94" t="s" s="15">
         <v>123</v>
       </c>
     </row>
-    <row r="90">
-      <c r="A90" t="s" s="17">
+    <row r="95">
+      <c r="A95" t="s" s="15">
         <v>124</v>
       </c>
     </row>
-    <row r="91">
-      <c r="A91" t="s" s="17">
+    <row r="96">
+      <c r="A96" t="s" s="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s" s="15">
         <v>125</v>
       </c>
     </row>
-    <row r="92">
-      <c r="A92" t="s" s="17">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s" s="17">
+    <row r="98">
+      <c r="A98" t="s" s="15">
         <v>126</v>
       </c>
     </row>
-    <row r="94">
-      <c r="A94" t="s" s="17">
+    <row r="99">
+      <c r="A99" t="s" s="15">
         <v>127</v>
       </c>
     </row>
-    <row r="95">
-      <c r="A95" t="s" s="17">
+    <row r="100">
+      <c r="A100" t="s" s="15">
         <v>128</v>
       </c>
     </row>
-    <row r="96">
-      <c r="A96" t="s" s="17">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s" s="17">
+    <row r="101">
+      <c r="A101" t="s" s="15">
         <v>129</v>
       </c>
     </row>
-    <row r="98">
-      <c r="A98" t="s" s="17">
+    <row r="102">
+      <c r="A102" t="s" s="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s" s="15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s" s="15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s" s="15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s" s="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s" s="15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s" s="15">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s" s="15">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s" s="15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s" s="15">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s" s="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s" s="15">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s" s="15">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s" s="15">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s" s="15">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s" s="15">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s" s="15">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s" s="15">
         <v>130</v>
       </c>
     </row>
-    <row r="99">
-      <c r="A99" t="s" s="17">
+    <row r="120">
+      <c r="A120" t="s" s="15">
         <v>131</v>
       </c>
     </row>
-    <row r="100">
-      <c r="A100" t="s" s="17">
+    <row r="121">
+      <c r="A121" t="s" s="15">
         <v>132</v>
       </c>
     </row>
-    <row r="101">
-      <c r="A101" t="s" s="17">
+    <row r="122">
+      <c r="A122" t="s" s="15">
         <v>133</v>
       </c>
     </row>
-    <row r="102">
-      <c r="A102" t="s" s="17">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s" s="17">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s" s="17">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s" s="17">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s" s="17">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s" s="17">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s" s="17">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="s" s="17">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="s" s="17">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="s" s="17">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" t="s" s="17">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" t="s" s="17">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" t="s" s="17">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" t="s" s="17">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" t="s" s="17">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" t="s" s="17">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" t="s" s="17">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="119">
-      <c r="A119" t="s" s="17">
+    <row r="123">
+      <c r="A123" t="s" s="15">
         <v>134</v>
       </c>
     </row>
-    <row r="120">
-      <c r="A120" t="s" s="17">
+    <row r="124">
+      <c r="A124" t="s" s="15">
         <v>135</v>
       </c>
     </row>
-    <row r="121">
-      <c r="A121" t="s" s="17">
+    <row r="125">
+      <c r="A125" t="s" s="15">
         <v>136</v>
       </c>
     </row>
-    <row r="122">
-      <c r="A122" t="s" s="17">
+    <row r="126">
+      <c r="A126" t="s" s="15">
         <v>137</v>
       </c>
     </row>
-    <row r="123">
-      <c r="A123" t="s" s="17">
+    <row r="127">
+      <c r="A127" t="s" s="15">
         <v>138</v>
       </c>
     </row>
-    <row r="124">
-      <c r="A124" t="s" s="17">
+    <row r="128">
+      <c r="A128" t="s" s="15">
         <v>139</v>
       </c>
     </row>
-    <row r="125">
-      <c r="A125" t="s" s="17">
+    <row r="129">
+      <c r="A129" t="s" s="15">
         <v>140</v>
       </c>
     </row>
-    <row r="126">
-      <c r="A126" t="s" s="17">
+    <row r="130">
+      <c r="A130" t="s" s="15">
         <v>141</v>
       </c>
     </row>
-    <row r="127">
-      <c r="A127" t="s" s="17">
+    <row r="131">
+      <c r="A131" t="s" s="15">
         <v>142</v>
       </c>
     </row>
-    <row r="128">
-      <c r="A128" t="s" s="17">
+    <row r="132">
+      <c r="A132" t="s" s="15">
         <v>143</v>
       </c>
     </row>
-    <row r="129">
-      <c r="A129" t="s" s="17">
+    <row r="133">
+      <c r="A133" t="s" s="15">
         <v>144</v>
       </c>
     </row>
-    <row r="130">
-      <c r="A130" t="s" s="17">
+    <row r="134">
+      <c r="A134" t="s" s="15">
         <v>145</v>
       </c>
     </row>
-    <row r="131">
-      <c r="A131" t="s" s="17">
+    <row r="135">
+      <c r="A135" t="s" s="15">
         <v>146</v>
       </c>
     </row>
-    <row r="132">
-      <c r="A132" t="s" s="17">
+    <row r="136">
+      <c r="A136" t="s" s="15">
         <v>147</v>
       </c>
     </row>
-    <row r="133">
-      <c r="A133" t="s" s="17">
+    <row r="137">
+      <c r="A137" t="s" s="15">
         <v>148</v>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" t="s" s="17">
+    <row r="138">
+      <c r="A138" t="s" s="15">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s" s="15">
         <v>149</v>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" t="s" s="17">
+    <row r="140">
+      <c r="A140" t="s" s="15">
         <v>150</v>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" t="s" s="17">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="s" s="17">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="s" s="17">
+    <row r="141">
+      <c r="A141" t="s" s="15">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="s" s="15">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="s" s="15">
         <v>76</v>
       </c>
     </row>
-    <row r="139">
-      <c r="A139" t="s" s="17">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="s" s="17">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="s" s="17">
+    <row r="144">
+      <c r="A144" t="s" s="15">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="s" s="15">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="s" s="15">
         <v>79</v>
       </c>
     </row>
-    <row r="142">
-      <c r="A142" t="s" s="17">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="s" s="17">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="s" s="17">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="s" s="17">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="s" s="17">
-        <v>79</v>
-      </c>
-    </row>
     <row r="147">
-      <c r="A147" t="s" s="17">
-        <v>89</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A66"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <cols>
-    <col min="1" max="1" width="255.0" customWidth="true" bestFit="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s" s="18">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s" s="19">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="19">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="19">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s" s="19">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s" s="19">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s" s="19">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="19">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="19">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s" s="19">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s" s="19">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s" s="19">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s" s="19">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s" s="19">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s" s="19">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s" s="19">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s" s="19">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s" s="19">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s" s="19">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s" s="19">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s" s="19">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s" s="19">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="19">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s" s="19">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s" s="19">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s" s="19">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="19">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s" s="19">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s" s="19">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s" s="19">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s" s="19">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="19">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s" s="19">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s" s="19">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s" s="19">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="19">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s" s="19">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s" s="19">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s" s="19">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s" s="19">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s" s="19">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s" s="19">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s" s="19">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s" s="19">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s" s="19">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s" s="19">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s" s="19">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s" s="19">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s" s="19">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s" s="19">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s" s="19">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s" s="19">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s" s="19">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s" s="19">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s" s="19">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s" s="19">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s" s="19">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s" s="19">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s" s="19">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s" s="19">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s" s="19">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s" s="19">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s" s="19">
+      <c r="A147" t="s" s="15">
         <v>89</v>
       </c>
     </row>

</xml_diff>